<commit_message>
edited the script w/ minor changes
</commit_message>
<xml_diff>
--- a/Clash.xlsx
+++ b/Clash.xlsx
@@ -4541,7 +4541,7 @@
   <dimension ref="A1:IV269"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -21788,7 +21788,7 @@
   <dimension ref="A1:IU316"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="C118" sqref="C118"/>
+      <selection activeCell="H110" sqref="H110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -22795,7 +22795,7 @@
         <v>16</v>
       </c>
       <c r="F29" s="71">
-        <f>235/E29</f>
+        <f t="shared" ref="F29:F42" si="0">235/E29</f>
         <v>14.6875</v>
       </c>
       <c r="G29" s="71" t="s">
@@ -22830,7 +22830,7 @@
         <v>17</v>
       </c>
       <c r="F30" s="71">
-        <f>235/E30</f>
+        <f t="shared" si="0"/>
         <v>13.823529411764707</v>
       </c>
       <c r="G30" s="71" t="s">
@@ -22865,7 +22865,7 @@
         <v>5</v>
       </c>
       <c r="F31" s="71">
-        <f>235/E31</f>
+        <f t="shared" si="0"/>
         <v>47</v>
       </c>
       <c r="G31" s="71" t="s">
@@ -22900,7 +22900,7 @@
         <v>14</v>
       </c>
       <c r="F32" s="71">
-        <f>235/E32</f>
+        <f t="shared" si="0"/>
         <v>16.785714285714285</v>
       </c>
       <c r="G32" s="71" t="s">
@@ -22935,7 +22935,7 @@
         <v>11</v>
       </c>
       <c r="F33" s="71">
-        <f>235/E33</f>
+        <f t="shared" si="0"/>
         <v>21.363636363636363</v>
       </c>
       <c r="G33" s="71" t="s">
@@ -22970,7 +22970,7 @@
         <v>4</v>
       </c>
       <c r="F34" s="71">
-        <f>235/E34</f>
+        <f t="shared" si="0"/>
         <v>58.75</v>
       </c>
       <c r="G34" s="71" t="s">
@@ -23005,7 +23005,7 @@
         <v>16</v>
       </c>
       <c r="F35" s="71">
-        <f>235/E35</f>
+        <f t="shared" si="0"/>
         <v>14.6875</v>
       </c>
       <c r="G35" s="71" t="s">
@@ -23040,7 +23040,7 @@
         <v>12</v>
       </c>
       <c r="F36" s="71">
-        <f>235/E36</f>
+        <f t="shared" si="0"/>
         <v>19.583333333333332</v>
       </c>
       <c r="G36" s="71" t="s">
@@ -23075,7 +23075,7 @@
         <v>1</v>
       </c>
       <c r="F37" s="71">
-        <f>235/E37</f>
+        <f t="shared" si="0"/>
         <v>235</v>
       </c>
       <c r="G37" s="71" t="s">
@@ -23110,7 +23110,7 @@
         <v>10</v>
       </c>
       <c r="F38" s="71">
-        <f>235/E38</f>
+        <f t="shared" si="0"/>
         <v>23.5</v>
       </c>
       <c r="G38" s="71" t="s">
@@ -23145,7 +23145,7 @@
         <v>8</v>
       </c>
       <c r="F39" s="71">
-        <f>235/E39</f>
+        <f t="shared" si="0"/>
         <v>29.375</v>
       </c>
       <c r="G39" s="71" t="s">
@@ -23180,7 +23180,7 @@
         <v>6</v>
       </c>
       <c r="F40" s="71">
-        <f>235/E40</f>
+        <f t="shared" si="0"/>
         <v>39.166666666666664</v>
       </c>
       <c r="G40" s="71" t="s">
@@ -23215,7 +23215,7 @@
         <v>7</v>
       </c>
       <c r="F41" s="71">
-        <f>235/E41</f>
+        <f t="shared" si="0"/>
         <v>33.571428571428569</v>
       </c>
       <c r="G41" s="71" t="s">
@@ -23250,7 +23250,7 @@
         <v>19</v>
       </c>
       <c r="F42" s="71">
-        <f>235/E42</f>
+        <f t="shared" si="0"/>
         <v>12.368421052631579</v>
       </c>
       <c r="G42" s="71" t="s">
@@ -23320,7 +23320,7 @@
         <v>16</v>
       </c>
       <c r="F44" s="71">
-        <f>235/E44</f>
+        <f t="shared" ref="F44:F52" si="1">235/E44</f>
         <v>14.6875</v>
       </c>
       <c r="G44" s="71" t="s">
@@ -23355,7 +23355,7 @@
         <v>7</v>
       </c>
       <c r="F45" s="71">
-        <f>235/E45</f>
+        <f t="shared" si="1"/>
         <v>33.571428571428569</v>
       </c>
       <c r="G45" s="71" t="s">
@@ -23390,7 +23390,7 @@
         <v>13</v>
       </c>
       <c r="F46" s="71">
-        <f>235/E46</f>
+        <f t="shared" si="1"/>
         <v>18.076923076923077</v>
       </c>
       <c r="G46" s="71" t="s">
@@ -23425,7 +23425,7 @@
         <v>2</v>
       </c>
       <c r="F47" s="71">
-        <f>235/E47</f>
+        <f t="shared" si="1"/>
         <v>117.5</v>
       </c>
       <c r="G47" s="71" t="s">
@@ -23460,7 +23460,7 @@
         <v>12</v>
       </c>
       <c r="F48" s="71">
-        <f>235/E48</f>
+        <f t="shared" si="1"/>
         <v>19.583333333333332</v>
       </c>
       <c r="G48" s="71" t="s">
@@ -23495,7 +23495,7 @@
         <v>8</v>
       </c>
       <c r="F49" s="71">
-        <f>235/E49</f>
+        <f t="shared" si="1"/>
         <v>29.375</v>
       </c>
       <c r="G49" s="71" t="s">
@@ -23530,7 +23530,7 @@
         <v>18</v>
       </c>
       <c r="F50" s="71">
-        <f>235/E50</f>
+        <f t="shared" si="1"/>
         <v>13.055555555555555</v>
       </c>
       <c r="G50" s="71" t="s">
@@ -23565,7 +23565,7 @@
         <v>4</v>
       </c>
       <c r="F51" s="71">
-        <f>235/E51</f>
+        <f t="shared" si="1"/>
         <v>58.75</v>
       </c>
       <c r="G51" s="71" t="s">
@@ -23600,7 +23600,7 @@
         <v>16</v>
       </c>
       <c r="F52" s="71">
-        <f>235/E52</f>
+        <f t="shared" si="1"/>
         <v>14.6875</v>
       </c>
       <c r="G52" s="71" t="s">
@@ -23775,7 +23775,7 @@
         <v>9</v>
       </c>
       <c r="F57" s="71">
-        <f>235/E57</f>
+        <f t="shared" ref="F57:F65" si="2">235/E57</f>
         <v>26.111111111111111</v>
       </c>
       <c r="G57" s="71" t="s">
@@ -23810,7 +23810,7 @@
         <v>7</v>
       </c>
       <c r="F58" s="71">
-        <f>235/E58</f>
+        <f t="shared" si="2"/>
         <v>33.571428571428569</v>
       </c>
       <c r="G58" s="71" t="s">
@@ -23845,7 +23845,7 @@
         <v>6</v>
       </c>
       <c r="F59" s="71">
-        <f>235/E59</f>
+        <f t="shared" si="2"/>
         <v>39.166666666666664</v>
       </c>
       <c r="G59" s="71" t="s">
@@ -23880,7 +23880,7 @@
         <v>15</v>
       </c>
       <c r="F60" s="71">
-        <f>235/E60</f>
+        <f t="shared" si="2"/>
         <v>15.666666666666666</v>
       </c>
       <c r="G60" s="71" t="s">
@@ -23915,7 +23915,7 @@
         <v>11</v>
       </c>
       <c r="F61" s="71">
-        <f>235/E61</f>
+        <f t="shared" si="2"/>
         <v>21.363636363636363</v>
       </c>
       <c r="G61" s="71" t="s">
@@ -23950,7 +23950,7 @@
         <v>19</v>
       </c>
       <c r="F62" s="71">
-        <f>235/E62</f>
+        <f t="shared" si="2"/>
         <v>12.368421052631579</v>
       </c>
       <c r="G62" s="71" t="s">
@@ -23985,7 +23985,7 @@
         <v>20</v>
       </c>
       <c r="F63" s="71">
-        <f>235/E63</f>
+        <f t="shared" si="2"/>
         <v>11.75</v>
       </c>
       <c r="G63" s="71" t="s">
@@ -24020,7 +24020,7 @@
         <v>8</v>
       </c>
       <c r="F64" s="71">
-        <f>235/E64</f>
+        <f t="shared" si="2"/>
         <v>29.375</v>
       </c>
       <c r="G64" s="71" t="s">
@@ -24055,7 +24055,7 @@
         <v>9</v>
       </c>
       <c r="F65" s="71">
-        <f>235/E65</f>
+        <f t="shared" si="2"/>
         <v>26.111111111111111</v>
       </c>
       <c r="G65" s="71" t="s">
@@ -24090,7 +24090,7 @@
         <v>1</v>
       </c>
       <c r="F66" s="71">
-        <f>77/E66</f>
+        <f t="shared" ref="F66:F71" si="3">77/E66</f>
         <v>77</v>
       </c>
       <c r="G66" s="71" t="s">
@@ -24125,7 +24125,7 @@
         <v>5</v>
       </c>
       <c r="F67" s="71">
-        <f>77/E67</f>
+        <f t="shared" si="3"/>
         <v>15.4</v>
       </c>
       <c r="G67" s="71" t="s">
@@ -24160,7 +24160,7 @@
         <v>3</v>
       </c>
       <c r="F68" s="71">
-        <f>77/E68</f>
+        <f t="shared" si="3"/>
         <v>25.666666666666668</v>
       </c>
       <c r="G68" s="71" t="s">
@@ -24195,7 +24195,7 @@
         <v>1</v>
       </c>
       <c r="F69" s="71">
-        <f>77/E69</f>
+        <f t="shared" si="3"/>
         <v>77</v>
       </c>
       <c r="G69" s="71" t="s">
@@ -24230,7 +24230,7 @@
         <v>9</v>
       </c>
       <c r="F70" s="71">
-        <f>77/E70</f>
+        <f t="shared" si="3"/>
         <v>8.5555555555555554</v>
       </c>
       <c r="G70" s="71" t="s">
@@ -24265,7 +24265,7 @@
         <v>2</v>
       </c>
       <c r="F71" s="71">
-        <f>77/E71</f>
+        <f t="shared" si="3"/>
         <v>38.5</v>
       </c>
       <c r="G71" s="71" t="s">
@@ -24300,7 +24300,7 @@
         <v>3</v>
       </c>
       <c r="F72" s="71">
-        <f>235/E72</f>
+        <f t="shared" ref="F72:F83" si="4">235/E72</f>
         <v>78.333333333333329</v>
       </c>
       <c r="G72" s="71" t="s">
@@ -24335,7 +24335,7 @@
         <v>5</v>
       </c>
       <c r="F73" s="71">
-        <f>235/E73</f>
+        <f t="shared" si="4"/>
         <v>47</v>
       </c>
       <c r="G73" s="71" t="s">
@@ -24370,7 +24370,7 @@
         <v>5</v>
       </c>
       <c r="F74" s="71">
-        <f>235/E74</f>
+        <f t="shared" si="4"/>
         <v>47</v>
       </c>
       <c r="G74" s="71" t="s">
@@ -24405,7 +24405,7 @@
         <v>7</v>
       </c>
       <c r="F75" s="71">
-        <f>235/E75</f>
+        <f t="shared" si="4"/>
         <v>33.571428571428569</v>
       </c>
       <c r="G75" s="71" t="s">
@@ -24440,7 +24440,7 @@
         <v>5</v>
       </c>
       <c r="F76" s="71">
-        <f>235/E76</f>
+        <f t="shared" si="4"/>
         <v>47</v>
       </c>
       <c r="G76" s="71" t="s">
@@ -24475,7 +24475,7 @@
         <v>20</v>
       </c>
       <c r="F77" s="71">
-        <f>235/E77</f>
+        <f t="shared" si="4"/>
         <v>11.75</v>
       </c>
       <c r="G77" s="71" t="s">
@@ -24510,7 +24510,7 @@
         <v>14</v>
       </c>
       <c r="F78" s="71">
-        <f>235/E78</f>
+        <f t="shared" si="4"/>
         <v>16.785714285714285</v>
       </c>
       <c r="G78" s="71" t="s">
@@ -24545,7 +24545,7 @@
         <v>14</v>
       </c>
       <c r="F79" s="71">
-        <f>235/E79</f>
+        <f t="shared" si="4"/>
         <v>16.785714285714285</v>
       </c>
       <c r="G79" s="71" t="s">
@@ -24580,7 +24580,7 @@
         <v>14</v>
       </c>
       <c r="F80" s="71">
-        <f>235/E80</f>
+        <f t="shared" si="4"/>
         <v>16.785714285714285</v>
       </c>
       <c r="G80" s="71" t="s">
@@ -24615,7 +24615,7 @@
         <v>7</v>
       </c>
       <c r="F81" s="71">
-        <f>235/E81</f>
+        <f t="shared" si="4"/>
         <v>33.571428571428569</v>
       </c>
       <c r="G81" s="71" t="s">
@@ -24650,7 +24650,7 @@
         <v>7</v>
       </c>
       <c r="F82" s="71">
-        <f>235/E82</f>
+        <f t="shared" si="4"/>
         <v>33.571428571428569</v>
       </c>
       <c r="G82" s="71" t="s">
@@ -24685,7 +24685,7 @@
         <v>14</v>
       </c>
       <c r="F83" s="71">
-        <f>235/E83</f>
+        <f t="shared" si="4"/>
         <v>16.785714285714285</v>
       </c>
       <c r="G83" s="71" t="s">
@@ -24790,7 +24790,7 @@
         <v>9</v>
       </c>
       <c r="F86" s="71">
-        <f>235/E86</f>
+        <f t="shared" ref="F86:F97" si="5">235/E86</f>
         <v>26.111111111111111</v>
       </c>
       <c r="G86" s="71" t="s">
@@ -24825,7 +24825,7 @@
         <v>5</v>
       </c>
       <c r="F87" s="71">
-        <f>235/E87</f>
+        <f t="shared" si="5"/>
         <v>47</v>
       </c>
       <c r="G87" s="71" t="s">
@@ -24860,7 +24860,7 @@
         <v>12</v>
       </c>
       <c r="F88" s="71">
-        <f>235/E88</f>
+        <f t="shared" si="5"/>
         <v>19.583333333333332</v>
       </c>
       <c r="G88" s="71" t="s">
@@ -24895,7 +24895,7 @@
         <v>9</v>
       </c>
       <c r="F89" s="71">
-        <f>235/E89</f>
+        <f t="shared" si="5"/>
         <v>26.111111111111111</v>
       </c>
       <c r="G89" s="71" t="s">
@@ -24930,7 +24930,7 @@
         <v>1</v>
       </c>
       <c r="F90" s="71">
-        <f>235/E90</f>
+        <f t="shared" si="5"/>
         <v>235</v>
       </c>
       <c r="G90" s="71" t="s">
@@ -24965,7 +24965,7 @@
         <v>3</v>
       </c>
       <c r="F91" s="71">
-        <f>235/E91</f>
+        <f t="shared" si="5"/>
         <v>78.333333333333329</v>
       </c>
       <c r="G91" s="71" t="s">
@@ -25000,7 +25000,7 @@
         <v>15</v>
       </c>
       <c r="F92" s="71">
-        <f>235/E92</f>
+        <f t="shared" si="5"/>
         <v>15.666666666666666</v>
       </c>
       <c r="G92" s="71" t="s">
@@ -25035,7 +25035,7 @@
         <v>8</v>
       </c>
       <c r="F93" s="71">
-        <f>235/E93</f>
+        <f t="shared" si="5"/>
         <v>29.375</v>
       </c>
       <c r="G93" s="71" t="s">
@@ -25070,7 +25070,7 @@
         <v>4</v>
       </c>
       <c r="F94" s="71">
-        <f>235/E94</f>
+        <f t="shared" si="5"/>
         <v>58.75</v>
       </c>
       <c r="G94" s="71" t="s">
@@ -25105,7 +25105,7 @@
         <v>6</v>
       </c>
       <c r="F95" s="71">
-        <f>235/E95</f>
+        <f t="shared" si="5"/>
         <v>39.166666666666664</v>
       </c>
       <c r="G95" s="71" t="s">
@@ -25140,7 +25140,7 @@
         <v>8</v>
       </c>
       <c r="F96" s="71">
-        <f>235/E96</f>
+        <f t="shared" si="5"/>
         <v>29.375</v>
       </c>
       <c r="G96" s="71" t="s">
@@ -25175,7 +25175,7 @@
         <v>8</v>
       </c>
       <c r="F97" s="71">
-        <f>235/E97</f>
+        <f t="shared" si="5"/>
         <v>29.375</v>
       </c>
       <c r="G97" s="71" t="s">
@@ -25350,7 +25350,7 @@
         <v>5</v>
       </c>
       <c r="F102" s="71">
-        <f>235/E102</f>
+        <f t="shared" ref="F102:F119" si="6">235/E102</f>
         <v>47</v>
       </c>
       <c r="G102" s="71" t="s">
@@ -25385,7 +25385,7 @@
         <v>1</v>
       </c>
       <c r="F103" s="71">
-        <f>235/E103</f>
+        <f t="shared" si="6"/>
         <v>235</v>
       </c>
       <c r="G103" s="71" t="s">
@@ -25420,7 +25420,7 @@
         <v>6</v>
       </c>
       <c r="F104" s="71">
-        <f>235/E104</f>
+        <f t="shared" si="6"/>
         <v>39.166666666666664</v>
       </c>
       <c r="G104" s="71" t="s">
@@ -25455,7 +25455,7 @@
         <v>13</v>
       </c>
       <c r="F105" s="71">
-        <f>235/E105</f>
+        <f t="shared" si="6"/>
         <v>18.076923076923077</v>
       </c>
       <c r="G105" s="71" t="s">
@@ -25490,7 +25490,7 @@
         <v>12</v>
       </c>
       <c r="F106" s="71">
-        <f>235/E106</f>
+        <f t="shared" si="6"/>
         <v>19.583333333333332</v>
       </c>
       <c r="G106" s="71" t="s">
@@ -25525,7 +25525,7 @@
         <v>4</v>
       </c>
       <c r="F107" s="71">
-        <f>235/E107</f>
+        <f t="shared" si="6"/>
         <v>58.75</v>
       </c>
       <c r="G107" s="71" t="s">
@@ -25560,7 +25560,7 @@
         <v>18</v>
       </c>
       <c r="F108" s="71">
-        <f>235/E108</f>
+        <f t="shared" si="6"/>
         <v>13.055555555555555</v>
       </c>
       <c r="G108" s="71" t="s">
@@ -25595,7 +25595,7 @@
         <v>16</v>
       </c>
       <c r="F109" s="71">
-        <f>235/E109</f>
+        <f t="shared" si="6"/>
         <v>14.6875</v>
       </c>
       <c r="G109" s="71" t="s">
@@ -25630,7 +25630,7 @@
         <v>19</v>
       </c>
       <c r="F110" s="71">
-        <f>235/E110</f>
+        <f t="shared" si="6"/>
         <v>12.368421052631579</v>
       </c>
       <c r="G110" s="71" t="s">
@@ -25665,7 +25665,7 @@
         <v>14</v>
       </c>
       <c r="F111" s="71">
-        <f>235/E111</f>
+        <f t="shared" si="6"/>
         <v>16.785714285714285</v>
       </c>
       <c r="G111" s="71" t="s">
@@ -25700,7 +25700,7 @@
         <v>8</v>
       </c>
       <c r="F112" s="71">
-        <f>235/E112</f>
+        <f t="shared" si="6"/>
         <v>29.375</v>
       </c>
       <c r="G112" s="71" t="s">
@@ -25735,7 +25735,7 @@
         <v>12</v>
       </c>
       <c r="F113" s="71">
-        <f>235/E113</f>
+        <f t="shared" si="6"/>
         <v>19.583333333333332</v>
       </c>
       <c r="G113" s="71" t="s">
@@ -25770,7 +25770,7 @@
         <v>4</v>
       </c>
       <c r="F114" s="71">
-        <f>235/E114</f>
+        <f t="shared" si="6"/>
         <v>58.75</v>
       </c>
       <c r="G114" s="71" t="s">
@@ -26046,7 +26046,7 @@
         <v>8</v>
       </c>
       <c r="F115" s="71">
-        <f>235/E115</f>
+        <f t="shared" si="6"/>
         <v>29.375</v>
       </c>
       <c r="G115" s="71" t="s">
@@ -26322,7 +26322,7 @@
         <v>10</v>
       </c>
       <c r="F116" s="71">
-        <f>235/E116</f>
+        <f t="shared" si="6"/>
         <v>23.5</v>
       </c>
       <c r="G116" s="71" t="s">
@@ -26598,7 +26598,7 @@
         <v>5</v>
       </c>
       <c r="F117" s="71">
-        <f>235/E117</f>
+        <f t="shared" si="6"/>
         <v>47</v>
       </c>
       <c r="G117" s="71" t="s">
@@ -26874,7 +26874,7 @@
         <v>1</v>
       </c>
       <c r="F118" s="71">
-        <f>235/E118</f>
+        <f t="shared" si="6"/>
         <v>235</v>
       </c>
       <c r="G118" s="71" t="s">
@@ -27150,7 +27150,7 @@
         <v>5</v>
       </c>
       <c r="F119" s="71">
-        <f>235/E119</f>
+        <f t="shared" si="6"/>
         <v>47</v>
       </c>
       <c r="G119" s="78"/>
@@ -27212,7 +27212,7 @@
         <v>18</v>
       </c>
       <c r="F121" s="71">
-        <f>235/E121</f>
+        <f t="shared" ref="F121:F128" si="7">235/E121</f>
         <v>13.055555555555555</v>
       </c>
       <c r="G121" s="71" t="s">
@@ -27244,7 +27244,7 @@
         <v>9</v>
       </c>
       <c r="F122" s="71">
-        <f>235/E122</f>
+        <f t="shared" si="7"/>
         <v>26.111111111111111</v>
       </c>
       <c r="G122" s="71" t="s">
@@ -27276,7 +27276,7 @@
         <v>17</v>
       </c>
       <c r="F123" s="71">
-        <f>235/E123</f>
+        <f t="shared" si="7"/>
         <v>13.823529411764707</v>
       </c>
       <c r="G123" s="71" t="s">
@@ -27308,7 +27308,7 @@
         <v>11</v>
       </c>
       <c r="F124" s="71">
-        <f>235/E124</f>
+        <f t="shared" si="7"/>
         <v>21.363636363636363</v>
       </c>
       <c r="G124" s="71" t="s">
@@ -27343,7 +27343,7 @@
         <v>16</v>
       </c>
       <c r="F125" s="71">
-        <f>235/E125</f>
+        <f t="shared" si="7"/>
         <v>14.6875</v>
       </c>
       <c r="G125" s="71" t="s">
@@ -27378,7 +27378,7 @@
         <v>10</v>
       </c>
       <c r="F126" s="71">
-        <f>235/E126</f>
+        <f t="shared" si="7"/>
         <v>23.5</v>
       </c>
       <c r="G126" s="71" t="s">
@@ -27413,7 +27413,7 @@
         <v>12</v>
       </c>
       <c r="F127" s="71">
-        <f>235/E127</f>
+        <f t="shared" si="7"/>
         <v>19.583333333333332</v>
       </c>
       <c r="G127" s="71" t="s">
@@ -27448,7 +27448,7 @@
         <v>11</v>
       </c>
       <c r="F128" s="71">
-        <f>235/E128</f>
+        <f t="shared" si="7"/>
         <v>21.363636363636363</v>
       </c>
       <c r="G128" s="71" t="s">
@@ -27798,7 +27798,7 @@
         <v>13</v>
       </c>
       <c r="F138" s="71">
-        <f>235/E138</f>
+        <f t="shared" ref="F138:F148" si="8">235/E138</f>
         <v>18.076923076923077</v>
       </c>
       <c r="G138" s="71" t="s">
@@ -27833,7 +27833,7 @@
         <v>10</v>
       </c>
       <c r="F139" s="71">
-        <f>235/E139</f>
+        <f t="shared" si="8"/>
         <v>23.5</v>
       </c>
       <c r="G139" s="71" t="s">
@@ -27868,7 +27868,7 @@
         <v>2</v>
       </c>
       <c r="F140" s="71">
-        <f>235/E140</f>
+        <f t="shared" si="8"/>
         <v>117.5</v>
       </c>
       <c r="G140" s="71" t="s">
@@ -27903,7 +27903,7 @@
         <v>6</v>
       </c>
       <c r="F141" s="71">
-        <f>235/E141</f>
+        <f t="shared" si="8"/>
         <v>39.166666666666664</v>
       </c>
       <c r="G141" s="71" t="s">
@@ -27938,7 +27938,7 @@
         <v>18</v>
       </c>
       <c r="F142" s="71">
-        <f>235/E142</f>
+        <f t="shared" si="8"/>
         <v>13.055555555555555</v>
       </c>
       <c r="G142" s="71" t="s">
@@ -27973,7 +27973,7 @@
         <v>6</v>
       </c>
       <c r="F143" s="71">
-        <f>235/E143</f>
+        <f t="shared" si="8"/>
         <v>39.166666666666664</v>
       </c>
       <c r="G143" s="71" t="s">
@@ -28008,7 +28008,7 @@
         <v>11</v>
       </c>
       <c r="F144" s="71">
-        <f>235/E144</f>
+        <f t="shared" si="8"/>
         <v>21.363636363636363</v>
       </c>
       <c r="G144" s="71" t="s">
@@ -28043,7 +28043,7 @@
         <v>6</v>
       </c>
       <c r="F145" s="71">
-        <f>235/E145</f>
+        <f t="shared" si="8"/>
         <v>39.166666666666664</v>
       </c>
       <c r="G145" s="71" t="s">
@@ -28078,7 +28078,7 @@
         <v>9</v>
       </c>
       <c r="F146" s="71">
-        <f>235/E146</f>
+        <f t="shared" si="8"/>
         <v>26.111111111111111</v>
       </c>
       <c r="G146" s="71" t="s">
@@ -28113,7 +28113,7 @@
         <v>4</v>
       </c>
       <c r="F147" s="71">
-        <f>235/E147</f>
+        <f t="shared" si="8"/>
         <v>58.75</v>
       </c>
       <c r="G147" s="71" t="s">
@@ -28148,7 +28148,7 @@
         <v>6</v>
       </c>
       <c r="F148" s="71">
-        <f>235/E148</f>
+        <f t="shared" si="8"/>
         <v>39.166666666666664</v>
       </c>
       <c r="G148" s="71" t="s">
@@ -28288,7 +28288,7 @@
         <v>15</v>
       </c>
       <c r="F152" s="71">
-        <f>235/E152</f>
+        <f t="shared" ref="F152:F187" si="9">235/E152</f>
         <v>15.666666666666666</v>
       </c>
       <c r="G152" s="71" t="s">
@@ -28323,7 +28323,7 @@
         <v>2</v>
       </c>
       <c r="F153" s="71">
-        <f>235/E153</f>
+        <f t="shared" si="9"/>
         <v>117.5</v>
       </c>
       <c r="G153" s="71" t="s">
@@ -28358,7 +28358,7 @@
         <v>7</v>
       </c>
       <c r="F154" s="71">
-        <f>235/E154</f>
+        <f t="shared" si="9"/>
         <v>33.571428571428569</v>
       </c>
       <c r="G154" s="71" t="s">
@@ -28393,7 +28393,7 @@
         <v>1</v>
       </c>
       <c r="F155" s="71">
-        <f>235/E155</f>
+        <f t="shared" si="9"/>
         <v>235</v>
       </c>
       <c r="G155" s="71" t="s">
@@ -28428,7 +28428,7 @@
         <v>3</v>
       </c>
       <c r="F156" s="71">
-        <f>235/E156</f>
+        <f t="shared" si="9"/>
         <v>78.333333333333329</v>
       </c>
       <c r="G156" s="71" t="s">
@@ -28463,7 +28463,7 @@
         <v>8</v>
       </c>
       <c r="F157" s="71">
-        <f>235/E157</f>
+        <f t="shared" si="9"/>
         <v>29.375</v>
       </c>
       <c r="G157" s="71" t="s">
@@ -28498,7 +28498,7 @@
         <v>10</v>
       </c>
       <c r="F158" s="71">
-        <f>235/E158</f>
+        <f t="shared" si="9"/>
         <v>23.5</v>
       </c>
       <c r="G158" s="71" t="s">
@@ -28533,7 +28533,7 @@
         <v>1</v>
       </c>
       <c r="F159" s="71">
-        <f>235/E159</f>
+        <f t="shared" si="9"/>
         <v>235</v>
       </c>
       <c r="G159" s="71" t="s">
@@ -28568,7 +28568,7 @@
         <v>3</v>
       </c>
       <c r="F160" s="71">
-        <f>235/E160</f>
+        <f t="shared" si="9"/>
         <v>78.333333333333329</v>
       </c>
       <c r="G160" s="71" t="s">
@@ -28603,7 +28603,7 @@
         <v>2</v>
       </c>
       <c r="F161" s="71">
-        <f>235/E161</f>
+        <f t="shared" si="9"/>
         <v>117.5</v>
       </c>
       <c r="G161" s="71" t="s">
@@ -28638,7 +28638,7 @@
         <v>5</v>
       </c>
       <c r="F162" s="71">
-        <f>235/E162</f>
+        <f t="shared" si="9"/>
         <v>47</v>
       </c>
       <c r="G162" s="71" t="s">
@@ -28673,7 +28673,7 @@
         <v>1</v>
       </c>
       <c r="F163" s="71">
-        <f>235/E163</f>
+        <f t="shared" si="9"/>
         <v>235</v>
       </c>
       <c r="G163" s="71" t="s">
@@ -28708,7 +28708,7 @@
         <v>13</v>
       </c>
       <c r="F164" s="71">
-        <f>235/E164</f>
+        <f t="shared" si="9"/>
         <v>18.076923076923077</v>
       </c>
       <c r="G164" s="71" t="s">
@@ -28743,7 +28743,7 @@
         <v>12</v>
       </c>
       <c r="F165" s="71">
-        <f>235/E165</f>
+        <f t="shared" si="9"/>
         <v>19.583333333333332</v>
       </c>
       <c r="G165" s="71" t="s">
@@ -28778,7 +28778,7 @@
         <v>5</v>
       </c>
       <c r="F166" s="71">
-        <f>235/E166</f>
+        <f t="shared" si="9"/>
         <v>47</v>
       </c>
       <c r="G166" s="71" t="s">
@@ -28813,7 +28813,7 @@
         <v>13</v>
       </c>
       <c r="F167" s="71">
-        <f>235/E167</f>
+        <f t="shared" si="9"/>
         <v>18.076923076923077</v>
       </c>
       <c r="G167" s="71" t="s">
@@ -28848,7 +28848,7 @@
         <v>11</v>
       </c>
       <c r="F168" s="71">
-        <f>235/E168</f>
+        <f t="shared" si="9"/>
         <v>21.363636363636363</v>
       </c>
       <c r="G168" s="71" t="s">
@@ -28883,7 +28883,7 @@
         <v>11</v>
       </c>
       <c r="F169" s="71">
-        <f>235/E169</f>
+        <f t="shared" si="9"/>
         <v>21.363636363636363</v>
       </c>
       <c r="G169" s="71" t="s">
@@ -28918,7 +28918,7 @@
         <v>3</v>
       </c>
       <c r="F170" s="71">
-        <f>235/E170</f>
+        <f t="shared" si="9"/>
         <v>78.333333333333329</v>
       </c>
       <c r="G170" s="71" t="s">
@@ -28953,7 +28953,7 @@
         <v>4</v>
       </c>
       <c r="F171" s="71">
-        <f>235/E171</f>
+        <f t="shared" si="9"/>
         <v>58.75</v>
       </c>
       <c r="G171" s="71" t="s">
@@ -28988,7 +28988,7 @@
         <v>1</v>
       </c>
       <c r="F172" s="71">
-        <f>235/E172</f>
+        <f t="shared" si="9"/>
         <v>235</v>
       </c>
       <c r="G172" s="71" t="s">
@@ -29023,7 +29023,7 @@
         <v>18</v>
       </c>
       <c r="F173" s="71">
-        <f>235/E173</f>
+        <f t="shared" si="9"/>
         <v>13.055555555555555</v>
       </c>
       <c r="G173" s="71" t="s">
@@ -29058,7 +29058,7 @@
         <v>3</v>
       </c>
       <c r="F174" s="71">
-        <f>235/E174</f>
+        <f t="shared" si="9"/>
         <v>78.333333333333329</v>
       </c>
       <c r="G174" s="71" t="s">
@@ -29093,7 +29093,7 @@
         <v>18</v>
       </c>
       <c r="F175" s="71">
-        <f>235/E175</f>
+        <f t="shared" si="9"/>
         <v>13.055555555555555</v>
       </c>
       <c r="G175" s="71" t="s">
@@ -29128,7 +29128,7 @@
         <v>13</v>
       </c>
       <c r="F176" s="71">
-        <f>235/E176</f>
+        <f t="shared" si="9"/>
         <v>18.076923076923077</v>
       </c>
       <c r="G176" s="71" t="s">
@@ -29163,7 +29163,7 @@
         <v>9</v>
       </c>
       <c r="F177" s="71">
-        <f>235/E177</f>
+        <f t="shared" si="9"/>
         <v>26.111111111111111</v>
       </c>
       <c r="G177" s="71" t="s">
@@ -29198,7 +29198,7 @@
         <v>7</v>
       </c>
       <c r="F178" s="71">
-        <f>235/E178</f>
+        <f t="shared" si="9"/>
         <v>33.571428571428569</v>
       </c>
       <c r="G178" s="71" t="s">
@@ -29233,7 +29233,7 @@
         <v>12</v>
       </c>
       <c r="F179" s="71">
-        <f>235/E179</f>
+        <f t="shared" si="9"/>
         <v>19.583333333333332</v>
       </c>
       <c r="G179" s="71" t="s">
@@ -29268,7 +29268,7 @@
         <v>3</v>
       </c>
       <c r="F180" s="71">
-        <f>235/E180</f>
+        <f t="shared" si="9"/>
         <v>78.333333333333329</v>
       </c>
       <c r="G180" s="71" t="s">
@@ -29303,7 +29303,7 @@
         <v>16</v>
       </c>
       <c r="F181" s="71">
-        <f>235/E181</f>
+        <f t="shared" si="9"/>
         <v>14.6875</v>
       </c>
       <c r="G181" s="71" t="s">
@@ -29338,7 +29338,7 @@
         <v>15</v>
       </c>
       <c r="F182" s="71">
-        <f>235/E182</f>
+        <f t="shared" si="9"/>
         <v>15.666666666666666</v>
       </c>
       <c r="G182" s="71" t="s">
@@ -29373,7 +29373,7 @@
         <v>1</v>
       </c>
       <c r="F183" s="71">
-        <f>235/E183</f>
+        <f t="shared" si="9"/>
         <v>235</v>
       </c>
       <c r="G183" s="71" t="s">
@@ -29408,7 +29408,7 @@
         <v>3</v>
       </c>
       <c r="F184" s="71">
-        <f>235/E184</f>
+        <f t="shared" si="9"/>
         <v>78.333333333333329</v>
       </c>
       <c r="G184" s="71" t="s">
@@ -29443,7 +29443,7 @@
         <v>10</v>
       </c>
       <c r="F185" s="71">
-        <f>235/E185</f>
+        <f t="shared" si="9"/>
         <v>23.5</v>
       </c>
       <c r="G185" s="71" t="s">
@@ -29478,7 +29478,7 @@
         <v>19</v>
       </c>
       <c r="F186" s="71">
-        <f>235/E186</f>
+        <f t="shared" si="9"/>
         <v>12.368421052631579</v>
       </c>
       <c r="G186" s="71" t="s">
@@ -29513,7 +29513,7 @@
         <v>12</v>
       </c>
       <c r="F187" s="71">
-        <f>235/E187</f>
+        <f t="shared" si="9"/>
         <v>19.583333333333332</v>
       </c>
       <c r="G187" s="71" t="s">
@@ -29863,7 +29863,7 @@
         <v>4</v>
       </c>
       <c r="F197" s="71">
-        <f>235/E197</f>
+        <f t="shared" ref="F197:F208" si="10">235/E197</f>
         <v>58.75</v>
       </c>
       <c r="G197" s="71" t="s">
@@ -29898,7 +29898,7 @@
         <v>11</v>
       </c>
       <c r="F198" s="71">
-        <f>235/E198</f>
+        <f t="shared" si="10"/>
         <v>21.363636363636363</v>
       </c>
       <c r="G198" s="71" t="s">
@@ -29933,7 +29933,7 @@
         <v>2</v>
       </c>
       <c r="F199" s="71">
-        <f>235/E199</f>
+        <f t="shared" si="10"/>
         <v>117.5</v>
       </c>
       <c r="G199" s="71" t="s">
@@ -29968,7 +29968,7 @@
         <v>3</v>
       </c>
       <c r="F200" s="71">
-        <f>235/E200</f>
+        <f t="shared" si="10"/>
         <v>78.333333333333329</v>
       </c>
       <c r="G200" s="71" t="s">
@@ -30003,7 +30003,7 @@
         <v>7</v>
       </c>
       <c r="F201" s="71">
-        <f>235/E201</f>
+        <f t="shared" si="10"/>
         <v>33.571428571428569</v>
       </c>
       <c r="G201" s="71" t="s">
@@ -30038,7 +30038,7 @@
         <v>2</v>
       </c>
       <c r="F202" s="71">
-        <f>235/E202</f>
+        <f t="shared" si="10"/>
         <v>117.5</v>
       </c>
       <c r="G202" s="71" t="s">
@@ -30073,7 +30073,7 @@
         <v>5</v>
       </c>
       <c r="F203" s="71">
-        <f>235/E203</f>
+        <f t="shared" si="10"/>
         <v>47</v>
       </c>
       <c r="G203" s="71" t="s">
@@ -30108,7 +30108,7 @@
         <v>17</v>
       </c>
       <c r="F204" s="71">
-        <f>235/E204</f>
+        <f t="shared" si="10"/>
         <v>13.823529411764707</v>
       </c>
       <c r="G204" s="71" t="s">
@@ -30143,7 +30143,7 @@
         <v>19</v>
       </c>
       <c r="F205" s="71">
-        <f>235/E205</f>
+        <f t="shared" si="10"/>
         <v>12.368421052631579</v>
       </c>
       <c r="G205" s="71" t="s">
@@ -30178,7 +30178,7 @@
         <v>5</v>
       </c>
       <c r="F206" s="71">
-        <f>235/E206</f>
+        <f t="shared" si="10"/>
         <v>47</v>
       </c>
       <c r="G206" s="71" t="s">
@@ -30213,7 +30213,7 @@
         <v>14</v>
       </c>
       <c r="F207" s="71">
-        <f>235/E207</f>
+        <f t="shared" si="10"/>
         <v>16.785714285714285</v>
       </c>
       <c r="G207" s="71" t="s">
@@ -30248,7 +30248,7 @@
         <v>13</v>
       </c>
       <c r="F208" s="71">
-        <f>235/E208</f>
+        <f t="shared" si="10"/>
         <v>18.076923076923077</v>
       </c>
       <c r="G208" s="71" t="s">
@@ -30353,7 +30353,7 @@
         <v>18</v>
       </c>
       <c r="F211" s="71">
-        <f>235/E211</f>
+        <f t="shared" ref="F211:F220" si="11">235/E211</f>
         <v>13.055555555555555</v>
       </c>
       <c r="G211" s="71" t="s">
@@ -30388,7 +30388,7 @@
         <v>8</v>
       </c>
       <c r="F212" s="71">
-        <f>235/E212</f>
+        <f t="shared" si="11"/>
         <v>29.375</v>
       </c>
       <c r="G212" s="71" t="s">
@@ -30423,7 +30423,7 @@
         <v>10</v>
       </c>
       <c r="F213" s="71">
-        <f>235/E213</f>
+        <f t="shared" si="11"/>
         <v>23.5</v>
       </c>
       <c r="G213" s="71" t="s">
@@ -30458,7 +30458,7 @@
         <v>7</v>
       </c>
       <c r="F214" s="71">
-        <f>235/E214</f>
+        <f t="shared" si="11"/>
         <v>33.571428571428569</v>
       </c>
       <c r="G214" s="71" t="s">
@@ -30493,7 +30493,7 @@
         <v>20</v>
       </c>
       <c r="F215" s="71">
-        <f>235/E215</f>
+        <f t="shared" si="11"/>
         <v>11.75</v>
       </c>
       <c r="G215" s="71" t="s">
@@ -30528,7 +30528,7 @@
         <v>10</v>
       </c>
       <c r="F216" s="71">
-        <f>235/E216</f>
+        <f t="shared" si="11"/>
         <v>23.5</v>
       </c>
       <c r="G216" s="71" t="s">
@@ -30563,7 +30563,7 @@
         <v>15</v>
       </c>
       <c r="F217" s="71">
-        <f>235/E217</f>
+        <f t="shared" si="11"/>
         <v>15.666666666666666</v>
       </c>
       <c r="G217" s="71" t="s">
@@ -30598,7 +30598,7 @@
         <v>8</v>
       </c>
       <c r="F218" s="71">
-        <f>235/E218</f>
+        <f t="shared" si="11"/>
         <v>29.375</v>
       </c>
       <c r="G218" s="71" t="s">
@@ -30633,7 +30633,7 @@
         <v>14</v>
       </c>
       <c r="F219" s="71">
-        <f>235/E219</f>
+        <f t="shared" si="11"/>
         <v>16.785714285714285</v>
       </c>
       <c r="G219" s="71" t="s">
@@ -30668,7 +30668,7 @@
         <v>8</v>
       </c>
       <c r="F220" s="71">
-        <f>235/E220</f>
+        <f t="shared" si="11"/>
         <v>29.375</v>
       </c>
       <c r="G220" s="71" t="s">
@@ -30738,7 +30738,7 @@
         <v>17</v>
       </c>
       <c r="F222" s="71">
-        <f>235/E222</f>
+        <f t="shared" ref="F222:F228" si="12">235/E222</f>
         <v>13.823529411764707</v>
       </c>
       <c r="G222" s="71" t="s">
@@ -30773,7 +30773,7 @@
         <v>1</v>
       </c>
       <c r="F223" s="71">
-        <f>235/E223</f>
+        <f t="shared" si="12"/>
         <v>235</v>
       </c>
       <c r="G223" s="71" t="s">
@@ -30808,7 +30808,7 @@
         <v>6</v>
       </c>
       <c r="F224" s="71">
-        <f>235/E224</f>
+        <f t="shared" si="12"/>
         <v>39.166666666666664</v>
       </c>
       <c r="G224" s="71" t="s">
@@ -30843,7 +30843,7 @@
         <v>10</v>
       </c>
       <c r="F225" s="71">
-        <f>235/E225</f>
+        <f t="shared" si="12"/>
         <v>23.5</v>
       </c>
       <c r="G225" s="71" t="s">
@@ -30878,7 +30878,7 @@
         <v>1</v>
       </c>
       <c r="F226" s="71">
-        <f>235/E226</f>
+        <f t="shared" si="12"/>
         <v>235</v>
       </c>
       <c r="G226" s="71" t="s">
@@ -30913,7 +30913,7 @@
         <v>11</v>
       </c>
       <c r="F227" s="71">
-        <f>235/E227</f>
+        <f t="shared" si="12"/>
         <v>21.363636363636363</v>
       </c>
       <c r="G227" s="71" t="s">
@@ -30948,7 +30948,7 @@
         <v>3</v>
       </c>
       <c r="F228" s="71">
-        <f>235/E228</f>
+        <f t="shared" si="12"/>
         <v>78.333333333333329</v>
       </c>
       <c r="G228" s="71" t="s">
@@ -31088,7 +31088,7 @@
         <v>13</v>
       </c>
       <c r="F232" s="71">
-        <f>77/E232</f>
+        <f t="shared" ref="F232:F238" si="13">77/E232</f>
         <v>5.9230769230769234</v>
       </c>
       <c r="G232" s="71" t="s">
@@ -31123,7 +31123,7 @@
         <v>2</v>
       </c>
       <c r="F233" s="71">
-        <f>77/E233</f>
+        <f t="shared" si="13"/>
         <v>38.5</v>
       </c>
       <c r="G233" s="71" t="s">
@@ -31158,7 +31158,7 @@
         <v>2</v>
       </c>
       <c r="F234" s="71">
-        <f>77/E234</f>
+        <f t="shared" si="13"/>
         <v>38.5</v>
       </c>
       <c r="G234" s="71" t="s">
@@ -31193,7 +31193,7 @@
         <v>2</v>
       </c>
       <c r="F235" s="71">
-        <f>77/E235</f>
+        <f t="shared" si="13"/>
         <v>38.5</v>
       </c>
       <c r="G235" s="71" t="s">
@@ -31228,7 +31228,7 @@
         <v>2</v>
       </c>
       <c r="F236" s="71">
-        <f>77/E236</f>
+        <f t="shared" si="13"/>
         <v>38.5</v>
       </c>
       <c r="G236" s="71" t="s">
@@ -31263,7 +31263,7 @@
         <v>1</v>
       </c>
       <c r="F237" s="71">
-        <f>77/E237</f>
+        <f t="shared" si="13"/>
         <v>77</v>
       </c>
       <c r="G237" s="71" t="s">
@@ -31298,7 +31298,7 @@
         <v>1</v>
       </c>
       <c r="F238" s="71">
-        <f>77/E238</f>
+        <f t="shared" si="13"/>
         <v>77</v>
       </c>
       <c r="G238" s="71" t="s">
@@ -31333,7 +31333,7 @@
         <v>19</v>
       </c>
       <c r="F239" s="71">
-        <f>235/E239</f>
+        <f t="shared" ref="F239:F245" si="14">235/E239</f>
         <v>12.368421052631579</v>
       </c>
       <c r="G239" s="71" t="s">
@@ -31368,7 +31368,7 @@
         <v>10</v>
       </c>
       <c r="F240" s="71">
-        <f>235/E240</f>
+        <f t="shared" si="14"/>
         <v>23.5</v>
       </c>
       <c r="G240" s="71" t="s">
@@ -31403,7 +31403,7 @@
         <v>12</v>
       </c>
       <c r="F241" s="71">
-        <f>235/E241</f>
+        <f t="shared" si="14"/>
         <v>19.583333333333332</v>
       </c>
       <c r="G241" s="71" t="s">
@@ -31438,7 +31438,7 @@
         <v>13</v>
       </c>
       <c r="F242" s="71">
-        <f>235/E242</f>
+        <f t="shared" si="14"/>
         <v>18.076923076923077</v>
       </c>
       <c r="G242" s="71" t="s">
@@ -31473,7 +31473,7 @@
         <v>14</v>
       </c>
       <c r="F243" s="71">
-        <f>235/E243</f>
+        <f t="shared" si="14"/>
         <v>16.785714285714285</v>
       </c>
       <c r="G243" s="71" t="s">
@@ -31508,7 +31508,7 @@
         <v>20</v>
       </c>
       <c r="F244" s="71">
-        <f>235/E244</f>
+        <f t="shared" si="14"/>
         <v>11.75</v>
       </c>
       <c r="G244" s="71" t="s">
@@ -31543,7 +31543,7 @@
         <v>2</v>
       </c>
       <c r="F245" s="71">
-        <f>235/E245</f>
+        <f t="shared" si="14"/>
         <v>117.5</v>
       </c>
       <c r="G245" s="71" t="s">
@@ -31578,7 +31578,7 @@
         <v>3</v>
       </c>
       <c r="F246" s="71">
-        <f>77/E246</f>
+        <f t="shared" ref="F246:F254" si="15">77/E246</f>
         <v>25.666666666666668</v>
       </c>
       <c r="G246" s="71" t="s">
@@ -31613,7 +31613,7 @@
         <v>2</v>
       </c>
       <c r="F247" s="71">
-        <f>77/E247</f>
+        <f t="shared" si="15"/>
         <v>38.5</v>
       </c>
       <c r="G247" s="71" t="s">
@@ -31648,7 +31648,7 @@
         <v>1</v>
       </c>
       <c r="F248" s="71">
-        <f>77/E248</f>
+        <f t="shared" si="15"/>
         <v>77</v>
       </c>
       <c r="G248" s="71" t="s">
@@ -31683,7 +31683,7 @@
         <v>3</v>
       </c>
       <c r="F249" s="71">
-        <f>77/E249</f>
+        <f t="shared" si="15"/>
         <v>25.666666666666668</v>
       </c>
       <c r="G249" s="71" t="s">
@@ -31718,7 +31718,7 @@
         <v>13</v>
       </c>
       <c r="F250" s="71">
-        <f>77/E250</f>
+        <f t="shared" si="15"/>
         <v>5.9230769230769234</v>
       </c>
       <c r="G250" s="71" t="s">
@@ -31753,7 +31753,7 @@
         <v>2</v>
       </c>
       <c r="F251" s="71">
-        <f>77/E251</f>
+        <f t="shared" si="15"/>
         <v>38.5</v>
       </c>
       <c r="G251" s="71" t="s">
@@ -31788,7 +31788,7 @@
         <v>4</v>
       </c>
       <c r="F252" s="71">
-        <f>77/E252</f>
+        <f t="shared" si="15"/>
         <v>19.25</v>
       </c>
       <c r="G252" s="71" t="s">
@@ -31823,7 +31823,7 @@
         <v>1</v>
       </c>
       <c r="F253" s="71">
-        <f>77/E253</f>
+        <f t="shared" si="15"/>
         <v>77</v>
       </c>
       <c r="G253" s="71" t="s">
@@ -31858,7 +31858,7 @@
         <v>7</v>
       </c>
       <c r="F254" s="71">
-        <f>77/E254</f>
+        <f t="shared" si="15"/>
         <v>11</v>
       </c>
       <c r="G254" s="71" t="s">
@@ -32138,7 +32138,7 @@
         <v>1</v>
       </c>
       <c r="F262" s="71">
-        <f>235/E262</f>
+        <f t="shared" ref="F262:F273" si="16">235/E262</f>
         <v>235</v>
       </c>
       <c r="G262" s="71" t="s">
@@ -32173,7 +32173,7 @@
         <v>3</v>
       </c>
       <c r="F263" s="71">
-        <f>235/E263</f>
+        <f t="shared" si="16"/>
         <v>78.333333333333329</v>
       </c>
       <c r="G263" s="71" t="s">
@@ -32208,7 +32208,7 @@
         <v>13</v>
       </c>
       <c r="F264" s="71">
-        <f>235/E264</f>
+        <f t="shared" si="16"/>
         <v>18.076923076923077</v>
       </c>
       <c r="G264" s="71" t="s">
@@ -32243,7 +32243,7 @@
         <v>4</v>
       </c>
       <c r="F265" s="71">
-        <f>235/E265</f>
+        <f t="shared" si="16"/>
         <v>58.75</v>
       </c>
       <c r="G265" s="71" t="s">
@@ -32278,7 +32278,7 @@
         <v>4</v>
       </c>
       <c r="F266" s="71">
-        <f>235/E266</f>
+        <f t="shared" si="16"/>
         <v>58.75</v>
       </c>
       <c r="G266" s="71" t="s">
@@ -32313,7 +32313,7 @@
         <v>15</v>
       </c>
       <c r="F267" s="71">
-        <f>235/E267</f>
+        <f t="shared" si="16"/>
         <v>15.666666666666666</v>
       </c>
       <c r="G267" s="71" t="s">
@@ -32348,7 +32348,7 @@
         <v>13</v>
       </c>
       <c r="F268" s="71">
-        <f>235/E268</f>
+        <f t="shared" si="16"/>
         <v>18.076923076923077</v>
       </c>
       <c r="G268" s="71" t="s">
@@ -32383,7 +32383,7 @@
         <v>2</v>
       </c>
       <c r="F269" s="71">
-        <f>235/E269</f>
+        <f t="shared" si="16"/>
         <v>117.5</v>
       </c>
       <c r="G269" s="71" t="s">
@@ -32418,7 +32418,7 @@
         <v>17</v>
       </c>
       <c r="F270" s="71">
-        <f>235/E270</f>
+        <f t="shared" si="16"/>
         <v>13.823529411764707</v>
       </c>
       <c r="G270" s="71" t="s">
@@ -32453,7 +32453,7 @@
         <v>3</v>
       </c>
       <c r="F271" s="71">
-        <f>235/E271</f>
+        <f t="shared" si="16"/>
         <v>78.333333333333329</v>
       </c>
       <c r="G271" s="71" t="s">
@@ -32488,7 +32488,7 @@
         <v>16</v>
       </c>
       <c r="F272" s="71">
-        <f>235/E272</f>
+        <f t="shared" si="16"/>
         <v>14.6875</v>
       </c>
       <c r="G272" s="71" t="s">
@@ -32523,7 +32523,7 @@
         <v>17</v>
       </c>
       <c r="F273" s="71">
-        <f>235/E273</f>
+        <f t="shared" si="16"/>
         <v>13.823529411764707</v>
       </c>
       <c r="G273" s="71" t="s">
@@ -32593,7 +32593,7 @@
         <v>15</v>
       </c>
       <c r="F275" s="71">
-        <f>235/E275</f>
+        <f t="shared" ref="F275:F280" si="17">235/E275</f>
         <v>15.666666666666666</v>
       </c>
       <c r="G275" s="71" t="s">
@@ -32628,7 +32628,7 @@
         <v>14</v>
       </c>
       <c r="F276" s="71">
-        <f>235/E276</f>
+        <f t="shared" si="17"/>
         <v>16.785714285714285</v>
       </c>
       <c r="G276" s="71" t="s">
@@ -32663,7 +32663,7 @@
         <v>11</v>
       </c>
       <c r="F277" s="71">
-        <f>235/E277</f>
+        <f t="shared" si="17"/>
         <v>21.363636363636363</v>
       </c>
       <c r="G277" s="71" t="s">
@@ -32698,7 +32698,7 @@
         <v>4</v>
       </c>
       <c r="F278" s="71">
-        <f>235/E278</f>
+        <f t="shared" si="17"/>
         <v>58.75</v>
       </c>
       <c r="G278" s="71" t="s">
@@ -32733,7 +32733,7 @@
         <v>9</v>
       </c>
       <c r="F279" s="71">
-        <f>235/E279</f>
+        <f t="shared" si="17"/>
         <v>26.111111111111111</v>
       </c>
       <c r="G279" s="71" t="s">
@@ -32768,7 +32768,7 @@
         <v>7</v>
       </c>
       <c r="F280" s="71">
-        <f>235/E280</f>
+        <f t="shared" si="17"/>
         <v>33.571428571428569</v>
       </c>
       <c r="G280" s="71" t="s">
@@ -33013,7 +33013,7 @@
         <v>4</v>
       </c>
       <c r="F287" s="71">
-        <f>77/E287</f>
+        <f t="shared" ref="F287:F293" si="18">77/E287</f>
         <v>19.25</v>
       </c>
       <c r="G287" s="71" t="s">
@@ -33048,7 +33048,7 @@
         <v>1</v>
       </c>
       <c r="F288" s="71">
-        <f>77/E288</f>
+        <f t="shared" si="18"/>
         <v>77</v>
       </c>
       <c r="G288" s="71" t="s">
@@ -33083,7 +33083,7 @@
         <v>1</v>
       </c>
       <c r="F289" s="71">
-        <f>77/E289</f>
+        <f t="shared" si="18"/>
         <v>77</v>
       </c>
       <c r="G289" s="71" t="s">
@@ -33118,7 +33118,7 @@
         <v>1</v>
       </c>
       <c r="F290" s="71">
-        <f>77/E290</f>
+        <f t="shared" si="18"/>
         <v>77</v>
       </c>
       <c r="G290" s="71" t="s">
@@ -33153,7 +33153,7 @@
         <v>3</v>
       </c>
       <c r="F291" s="71">
-        <f>77/E291</f>
+        <f t="shared" si="18"/>
         <v>25.666666666666668</v>
       </c>
       <c r="G291" s="71" t="s">
@@ -33188,7 +33188,7 @@
         <v>1</v>
       </c>
       <c r="F292" s="71">
-        <f>77/E292</f>
+        <f t="shared" si="18"/>
         <v>77</v>
       </c>
       <c r="G292" s="71" t="s">
@@ -33223,7 +33223,7 @@
         <v>3</v>
       </c>
       <c r="F293" s="71">
-        <f>77/E293</f>
+        <f t="shared" si="18"/>
         <v>25.666666666666668</v>
       </c>
       <c r="G293" s="71" t="s">
@@ -33258,7 +33258,7 @@
         <v>13</v>
       </c>
       <c r="F294" s="71">
-        <f>235/E294</f>
+        <f t="shared" ref="F294:F303" si="19">235/E294</f>
         <v>18.076923076923077</v>
       </c>
       <c r="G294" s="71" t="s">
@@ -33293,7 +33293,7 @@
         <v>9</v>
       </c>
       <c r="F295" s="71">
-        <f>235/E295</f>
+        <f t="shared" si="19"/>
         <v>26.111111111111111</v>
       </c>
       <c r="G295" s="71" t="s">
@@ -33328,7 +33328,7 @@
         <v>20</v>
       </c>
       <c r="F296" s="71">
-        <f>235/E296</f>
+        <f t="shared" si="19"/>
         <v>11.75</v>
       </c>
       <c r="G296" s="71" t="s">
@@ -33363,7 +33363,7 @@
         <v>15</v>
       </c>
       <c r="F297" s="71">
-        <f>235/E297</f>
+        <f t="shared" si="19"/>
         <v>15.666666666666666</v>
       </c>
       <c r="G297" s="71" t="s">
@@ -33398,7 +33398,7 @@
         <v>7</v>
       </c>
       <c r="F298" s="71">
-        <f>235/E298</f>
+        <f t="shared" si="19"/>
         <v>33.571428571428569</v>
       </c>
       <c r="G298" s="71" t="s">
@@ -33433,7 +33433,7 @@
         <v>9</v>
       </c>
       <c r="F299" s="71">
-        <f>235/E299</f>
+        <f t="shared" si="19"/>
         <v>26.111111111111111</v>
       </c>
       <c r="G299" s="71" t="s">
@@ -33468,7 +33468,7 @@
         <v>5</v>
       </c>
       <c r="F300" s="71">
-        <f>235/E300</f>
+        <f t="shared" si="19"/>
         <v>47</v>
       </c>
       <c r="G300" s="71" t="s">
@@ -33503,7 +33503,7 @@
         <v>2</v>
       </c>
       <c r="F301" s="71">
-        <f>235/E301</f>
+        <f t="shared" si="19"/>
         <v>117.5</v>
       </c>
       <c r="G301" s="71" t="s">
@@ -33538,7 +33538,7 @@
         <v>2</v>
       </c>
       <c r="F302" s="71">
-        <f>235/E302</f>
+        <f t="shared" si="19"/>
         <v>117.5</v>
       </c>
       <c r="G302" s="71" t="s">
@@ -33573,7 +33573,7 @@
         <v>2</v>
       </c>
       <c r="F303" s="71">
-        <f>235/E303</f>
+        <f t="shared" si="19"/>
         <v>117.5</v>
       </c>
       <c r="G303" s="71" t="s">

</xml_diff>